<commit_message>
refactor(sheet) : refactor the function column_set_answer_in_group to put in input a synthetical dictionary, create a function to automatically reverse dictionaries in utils.py.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -513,6 +513,106 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="Y1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="Z1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -555,12 +655,112 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="N2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Q2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="R2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="T2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="U2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="V2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="X2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Y2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Z2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AC2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J2" s="5" t="n"/>
+      <c r="AD2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -603,12 +803,112 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Q3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="R3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="S3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="T3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="U3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="V3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="W3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="X3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Y3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Z3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AC3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J3" s="5" t="n"/>
+      <c r="AD3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -651,12 +951,112 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="R4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="T4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="U4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="V4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="X4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Y4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Z4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AC4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J4" s="5" t="n"/>
+      <c r="AD4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -699,12 +1099,112 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="P5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Q5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="R5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="T5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="U5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="V5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="X5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Y5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Z5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AC5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J5" s="5" t="n"/>
+      <c r="AD5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -747,12 +1247,112 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="P6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="T6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="U6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="V6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="X6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Y6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="Z6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AC6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J6" s="5" t="n"/>
+      <c r="AD6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -795,12 +1395,112 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="P7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="R7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="T7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="U7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="V7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="X7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Y7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Z7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AC7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J7" s="5" t="n"/>
+      <c r="AD7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -843,12 +1543,112 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="I8" s="5" t="inlineStr">
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="P8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="R8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="T8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="U8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="V8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="X8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Y8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Z8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AC8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J8" s="5" t="n"/>
+      <c r="AD8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -891,12 +1691,112 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr">
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="O9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="P9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Q9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="R9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="S9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="T9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="U9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="V9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="W9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="X9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Y9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="Z9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AC9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="J9" s="5" t="n"/>
+      <c r="AD9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
style(all) : lintering all the code with ruff
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:ADB9"/>
+  <dimension ref="A1:ADF9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -4373,6 +4373,26 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="ADA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ADB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ADC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ADD1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -8275,12 +8295,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ADA2" s="5" t="inlineStr">
+      <c r="ADA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADD2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADE2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB2" s="5" t="n"/>
+      <c r="ADF2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -12183,12 +12223,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ADA3" s="5" t="inlineStr">
+      <c r="ADA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADE3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB3" s="5" t="n"/>
+      <c r="ADF3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -16091,12 +16151,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ADA4" s="5" t="inlineStr">
+      <c r="ADA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADE4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB4" s="5" t="n"/>
+      <c r="ADF4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -19999,12 +20079,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ADA5" s="5" t="inlineStr">
+      <c r="ADA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADD5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADE5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB5" s="5" t="n"/>
+      <c r="ADF5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -23907,12 +24007,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ADA6" s="5" t="inlineStr">
+      <c r="ADA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADD6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADE6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB6" s="5" t="n"/>
+      <c r="ADF6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -27815,12 +27935,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ADA7" s="5" t="inlineStr">
+      <c r="ADA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADE7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB7" s="5" t="n"/>
+      <c r="ADF7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -31723,12 +31863,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ADA8" s="5" t="inlineStr">
+      <c r="ADA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ADD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADE8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB8" s="5" t="n"/>
+      <c r="ADF8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -35631,12 +35791,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ADA9" s="5" t="inlineStr">
+      <c r="ADA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ADE9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ADB9" s="5" t="n"/>
+      <c r="ADF9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat(module_pour_excel): modify create_one_onglet_by_participant to write data on an other file
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AFN9"/>
+  <dimension ref="A1:AFV9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -4693,6 +4693,46 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AFM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AFN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AFO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AFP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AFQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AFR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AFS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AFT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -8915,12 +8955,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFM2" s="5" t="inlineStr">
+      <c r="AFM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFU2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN2" s="5" t="n"/>
+      <c r="AFV2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -13143,12 +13223,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFM3" s="5" t="inlineStr">
+      <c r="AFM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFU3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN3" s="5" t="n"/>
+      <c r="AFV3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -17371,12 +17491,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFM4" s="5" t="inlineStr">
+      <c r="AFM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFU4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN4" s="5" t="n"/>
+      <c r="AFV4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -21599,12 +21759,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFM5" s="5" t="inlineStr">
+      <c r="AFM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFU5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN5" s="5" t="n"/>
+      <c r="AFV5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -25827,12 +26027,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFM6" s="5" t="inlineStr">
+      <c r="AFM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFU6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN6" s="5" t="n"/>
+      <c r="AFV6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -30055,12 +30295,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFM7" s="5" t="inlineStr">
+      <c r="AFM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFU7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN7" s="5" t="n"/>
+      <c r="AFV7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -34283,12 +34563,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFM8" s="5" t="inlineStr">
+      <c r="AFM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFU8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN8" s="5" t="n"/>
+      <c r="AFV8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -38511,12 +38831,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFM9" s="5" t="inlineStr">
+      <c r="AFM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFU9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFN9" s="5" t="n"/>
+      <c r="AFV9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat,test(create_one_onglet_by_participant): modify this method to register tabs in a different file and modify the associated unitary test
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AFV9"/>
+  <dimension ref="A1:AIL9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -4733,6 +4733,346 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AFU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AFV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AFW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AFX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AFY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AFZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGD1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGE1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGI1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGL1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGN1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AGW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AGX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AGY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AGZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHD1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHE1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHF1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHG1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHH1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHI1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHJ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHK1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHL1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AHW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AHX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AHY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AHZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AIC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AID1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIE1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AIG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AIH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AII1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -8995,12 +9335,352 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFU2" s="5" t="inlineStr">
+      <c r="AFU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGD2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGL2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGN2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHD2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHF2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHH2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHJ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHL2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AID2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIK2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV2" s="5" t="n"/>
+      <c r="AIL2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -13263,12 +13943,352 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFU3" s="5" t="inlineStr">
+      <c r="AFU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AID3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AII3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIK3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV3" s="5" t="n"/>
+      <c r="AIL3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -17531,12 +18551,352 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFU4" s="5" t="inlineStr">
+      <c r="AFU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AID4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIK4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV4" s="5" t="n"/>
+      <c r="AIL4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -21799,12 +23159,352 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFU5" s="5" t="inlineStr">
+      <c r="AFU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGD5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGL5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGN5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHD5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHF5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHH5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHJ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHL5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AID5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIK5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV5" s="5" t="n"/>
+      <c r="AIL5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -26067,12 +27767,352 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AFU6" s="5" t="inlineStr">
+      <c r="AFU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGD6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGL6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGN6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHD6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHF6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHH6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHJ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHL6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AID6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIK6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV6" s="5" t="n"/>
+      <c r="AIL6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -30335,12 +32375,352 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFU7" s="5" t="inlineStr">
+      <c r="AFU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AID7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIK7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV7" s="5" t="n"/>
+      <c r="AIL7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -34603,12 +36983,352 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFU8" s="5" t="inlineStr">
+      <c r="AFU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AFX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AGZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHE8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHI8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AHX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AID8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIK8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV8" s="5" t="n"/>
+      <c r="AIL8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -38871,12 +41591,352 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AFU9" s="5" t="inlineStr">
+      <c r="AFU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AFZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AGZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AHZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AID9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AII9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIK9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AFV9" s="5" t="n"/>
+      <c r="AIL9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
test(module_pour_excel): test for create_oneongletbyparticipant method of Path
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AIL9"/>
+  <dimension ref="A1:AKD9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5073,6 +5073,226 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AIK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AIL1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIN1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AIO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AIP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AIS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AIT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AIW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AIX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AIY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AIZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJD1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJE1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJF1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJG1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJH1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJI1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJJ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJK1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJL1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AJW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AJX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AJY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AJZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -9675,12 +9895,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AIK2" s="5" t="inlineStr">
+      <c r="AIK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIL2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIN2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJD2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJF2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJH2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJJ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJL2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKC2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL2" s="5" t="n"/>
+      <c r="AKD2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -14283,12 +14723,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AIK3" s="5" t="inlineStr">
+      <c r="AIK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKC3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL3" s="5" t="n"/>
+      <c r="AKD3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -18891,12 +19551,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AIK4" s="5" t="inlineStr">
+      <c r="AIK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKC4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL4" s="5" t="n"/>
+      <c r="AKD4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -23499,12 +24379,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AIK5" s="5" t="inlineStr">
+      <c r="AIK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIL5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIN5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJD5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJF5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJH5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJJ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJL5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKC5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL5" s="5" t="n"/>
+      <c r="AKD5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -28107,12 +29207,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AIK6" s="5" t="inlineStr">
+      <c r="AIK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIL6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIN6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJD6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJF6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJH6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJJ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJL6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKC6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL6" s="5" t="n"/>
+      <c r="AKD6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -32715,12 +34035,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AIK7" s="5" t="inlineStr">
+      <c r="AIK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKC7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL7" s="5" t="n"/>
+      <c r="AKD7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -37323,12 +38863,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AIK8" s="5" t="inlineStr">
+      <c r="AIK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AIZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJE8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJI8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AJX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKC8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL8" s="5" t="n"/>
+      <c r="AKD8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -41931,12 +43691,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AIK9" s="5" t="inlineStr">
+      <c r="AIK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AIZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AJZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKC9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AIL9" s="5" t="n"/>
+      <c r="AKD9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat,test(module_pour_excel): write a method check_linenumber_of_tabs and a test
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AKD9"/>
+  <dimension ref="A1:AKP9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5293,6 +5293,66 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AKC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKD1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKE1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AKG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKI1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AKK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKL1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKN1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -10115,12 +10175,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKC2" s="5" t="inlineStr">
+      <c r="AKC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKD2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKL2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKN2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKO2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD2" s="5" t="n"/>
+      <c r="AKP2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -14943,12 +15063,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKC3" s="5" t="inlineStr">
+      <c r="AKC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKO3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD3" s="5" t="n"/>
+      <c r="AKP3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -19771,12 +19951,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKC4" s="5" t="inlineStr">
+      <c r="AKC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKO4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD4" s="5" t="n"/>
+      <c r="AKP4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -24599,12 +24839,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKC5" s="5" t="inlineStr">
+      <c r="AKC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKD5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKL5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKN5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKO5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD5" s="5" t="n"/>
+      <c r="AKP5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -29427,12 +29727,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKC6" s="5" t="inlineStr">
+      <c r="AKC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKD6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKL6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKN6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKO6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD6" s="5" t="n"/>
+      <c r="AKP6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -34255,12 +34615,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKC7" s="5" t="inlineStr">
+      <c r="AKC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKO7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD7" s="5" t="n"/>
+      <c r="AKP7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -39083,12 +39503,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKC8" s="5" t="inlineStr">
+      <c r="AKC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKO8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD8" s="5" t="n"/>
+      <c r="AKP8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -43911,12 +44391,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKC9" s="5" t="inlineStr">
+      <c r="AKC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKO9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKD9" s="5" t="n"/>
+      <c r="AKP9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
test,feat(xlspython): test two functions created in the last commit and write commands for it, colgetbegin, maptwocols
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AKP9"/>
+  <dimension ref="A1:ALZ9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5353,6 +5353,186 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AKO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AKS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AKW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AKX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AKY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AKZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALD1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALE1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALF1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALG1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALH1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALI1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALJ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALK1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALL1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ALU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ALW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ALX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -10235,12 +10415,192 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKO2" s="5" t="inlineStr">
+      <c r="AKO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALD2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALF2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALH2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALJ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALL2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALY2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP2" s="5" t="n"/>
+      <c r="ALZ2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -15123,12 +15483,192 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKO3" s="5" t="inlineStr">
+      <c r="AKO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALY3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP3" s="5" t="n"/>
+      <c r="ALZ3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -20011,12 +20551,192 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKO4" s="5" t="inlineStr">
+      <c r="AKO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALY4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP4" s="5" t="n"/>
+      <c r="ALZ4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -24899,12 +25619,192 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKO5" s="5" t="inlineStr">
+      <c r="AKO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALD5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALF5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALH5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALJ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALL5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALY5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP5" s="5" t="n"/>
+      <c r="ALZ5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -29787,12 +30687,192 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AKO6" s="5" t="inlineStr">
+      <c r="AKO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALD6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALF6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALH6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALJ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALL6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALY6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP6" s="5" t="n"/>
+      <c r="ALZ6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -34675,12 +35755,192 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKO7" s="5" t="inlineStr">
+      <c r="AKO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALY7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP7" s="5" t="n"/>
+      <c r="ALZ7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -39563,12 +40823,192 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKO8" s="5" t="inlineStr">
+      <c r="AKO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AKZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALE8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALI8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALY8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP8" s="5" t="n"/>
+      <c r="ALZ8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -44451,12 +45891,192 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AKO9" s="5" t="inlineStr">
+      <c r="AKO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AKZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALY9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AKP9" s="5" t="n"/>
+      <c r="ALZ9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat, test(xlspython): test de extract_cells_from_all_sheets et écriture de la commande associée
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:ALZ9"/>
+  <dimension ref="A1:ANV9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5533,6 +5533,246 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="ALY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ALZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AMD1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AME1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AMH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMI1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AML1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMN1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AMP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AMT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AMW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AMX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AMY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AMZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ANA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ANB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ANC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AND1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ANE1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ANF1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ANG1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ANH1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ANI1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ANJ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ANK1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ANL1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ANM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ANN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ANO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ANP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ANQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ANR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ANS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ANT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -10595,12 +10835,252 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ALY2" s="5" t="inlineStr">
+      <c r="ALY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMD2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AML2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMN2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AND2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANF2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANH2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANJ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANL2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANU2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ2" s="5" t="n"/>
+      <c r="ANV2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -15663,12 +16143,252 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ALY3" s="5" t="inlineStr">
+      <c r="ALY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AME3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AML3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AND3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANU3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ3" s="5" t="n"/>
+      <c r="ANV3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -20731,12 +21451,252 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ALY4" s="5" t="inlineStr">
+      <c r="ALY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AML4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AND4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANU4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ4" s="5" t="n"/>
+      <c r="ANV4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -25799,12 +26759,252 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ALY5" s="5" t="inlineStr">
+      <c r="ALY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMD5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AML5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMN5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AND5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANF5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANH5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANJ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANL5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANU5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ5" s="5" t="n"/>
+      <c r="ANV5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -30867,12 +32067,252 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ALY6" s="5" t="inlineStr">
+      <c r="ALY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ALZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMD6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AML6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMN6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AND6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANF6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANH6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANJ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANL6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANU6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ6" s="5" t="n"/>
+      <c r="ANV6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -35935,12 +37375,252 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ALY7" s="5" t="inlineStr">
+      <c r="ALY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AML7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AND7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANU7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ7" s="5" t="n"/>
+      <c r="ANV7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -41003,12 +42683,252 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ALY8" s="5" t="inlineStr">
+      <c r="ALY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AML8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AMZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AND8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANE8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANI8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ANT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANU8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ8" s="5" t="n"/>
+      <c r="ANV8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -46071,12 +47991,252 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ALY9" s="5" t="inlineStr">
+      <c r="ALY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ALZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AME9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AML9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AMZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AND9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ANU9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ALZ9" s="5" t="n"/>
+      <c r="ANV9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
factor(all): delete the insert boolean. Now, nothing writes on already written cells
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AOL9"/>
+  <dimension ref="A1:AOT9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5853,6 +5853,46 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AOK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AOL1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AOM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AON1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AOO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AOP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AOQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AOR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -11235,12 +11275,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOK2" s="5" t="inlineStr">
+      <c r="AOK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOL2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AON2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOS2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL2" s="5" t="n"/>
+      <c r="AOT2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -16623,12 +16703,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOK3" s="5" t="inlineStr">
+      <c r="AOK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AON3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOS3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL3" s="5" t="n"/>
+      <c r="AOT3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -22011,12 +22131,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOK4" s="5" t="inlineStr">
+      <c r="AOK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AON4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOS4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL4" s="5" t="n"/>
+      <c r="AOT4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -27399,12 +27559,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOK5" s="5" t="inlineStr">
+      <c r="AOK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOL5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AON5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOS5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL5" s="5" t="n"/>
+      <c r="AOT5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -32787,12 +32987,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOK6" s="5" t="inlineStr">
+      <c r="AOK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOL6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AON6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOS6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL6" s="5" t="n"/>
+      <c r="AOT6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -38175,12 +38415,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOK7" s="5" t="inlineStr">
+      <c r="AOK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AON7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOS7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL7" s="5" t="n"/>
+      <c r="AOT7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -43563,12 +43843,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOK8" s="5" t="inlineStr">
+      <c r="AOK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AON8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOS8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL8" s="5" t="n"/>
+      <c r="AOT8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -48951,12 +49271,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOK9" s="5" t="inlineStr">
+      <c r="AOK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AON9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOS9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOL9" s="5" t="n"/>
+      <c r="AOT9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat(module_pour_excel): write and test a decorator act_on_columns which reduces the function to the loop. The decorator transforms column letters in indexes, apply the function, update formulas and save the file
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AOT9"/>
+  <dimension ref="A1:APB9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -5893,6 +5893,46 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AOS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AOT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AOU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AOV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AOW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AOX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AOY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AOZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -11315,12 +11355,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOS2" s="5" t="inlineStr">
+      <c r="AOS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APA2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT2" s="5" t="n"/>
+      <c r="APB2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -16743,12 +16823,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOS3" s="5" t="inlineStr">
+      <c r="AOS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APA3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT3" s="5" t="n"/>
+      <c r="APB3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -22171,12 +22291,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOS4" s="5" t="inlineStr">
+      <c r="AOS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APA4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT4" s="5" t="n"/>
+      <c r="APB4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -27599,12 +27759,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOS5" s="5" t="inlineStr">
+      <c r="AOS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APA5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT5" s="5" t="n"/>
+      <c r="APB5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -33027,12 +33227,52 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AOS6" s="5" t="inlineStr">
+      <c r="AOS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APA6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT6" s="5" t="n"/>
+      <c r="APB6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -38455,12 +38695,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOS7" s="5" t="inlineStr">
+      <c r="AOS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APA7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT7" s="5" t="n"/>
+      <c r="APB7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -43883,12 +44163,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOS8" s="5" t="inlineStr">
+      <c r="AOS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AOZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APA8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT8" s="5" t="n"/>
+      <c r="APB8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -49311,12 +49631,52 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AOS9" s="5" t="inlineStr">
+      <c r="AOS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AOZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APA9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AOT9" s="5" t="n"/>
+      <c r="APB9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
factor(module_pour_excel): clean all commented odl methods prior to the add of the descriptor act_on_columns
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:APV9"/>
+  <dimension ref="A1:APZ9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -6033,6 +6033,26 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="APU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="APV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="APW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="APX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -11595,12 +11615,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APU2" s="5" t="inlineStr">
+      <c r="APU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APY2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV2" s="5" t="n"/>
+      <c r="APZ2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -17163,12 +17203,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APU3" s="5" t="inlineStr">
+      <c r="APU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APY3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV3" s="5" t="n"/>
+      <c r="APZ3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -22731,12 +22791,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APU4" s="5" t="inlineStr">
+      <c r="APU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APY4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV4" s="5" t="n"/>
+      <c r="APZ4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -28299,12 +28379,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APU5" s="5" t="inlineStr">
+      <c r="APU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APY5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV5" s="5" t="n"/>
+      <c r="APZ5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -33867,12 +33967,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APU6" s="5" t="inlineStr">
+      <c r="APU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APY6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV6" s="5" t="n"/>
+      <c r="APZ6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -39435,12 +39555,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APU7" s="5" t="inlineStr">
+      <c r="APU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APY7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV7" s="5" t="n"/>
+      <c r="APZ7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -45003,12 +45143,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APU8" s="5" t="inlineStr">
+      <c r="APU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APY8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV8" s="5" t="n"/>
+      <c r="APZ8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -50571,12 +50731,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APU9" s="5" t="inlineStr">
+      <c r="APU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APY9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APV9" s="5" t="n"/>
+      <c r="APZ9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat(module_pour_excel): write the method apply_method_on_all_sheets in File to apply one method of Sheet on all tabs
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:APZ9"/>
+  <dimension ref="A1:ARR9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -6053,6 +6053,226 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="APY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="APZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQD1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQE1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQI1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQK1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQL1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQM1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQN1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQO1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQP1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQQ1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQR1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQS1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQT1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQU1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQV1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="AQW1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AQX1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AQY1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AQZ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARA1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARB1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARC1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ARD1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARE1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARF1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARG1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ARH1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARI1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARJ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARK1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ARL1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ARP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -11635,12 +11855,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APY2" s="5" t="inlineStr">
+      <c r="APY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQD2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQL2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQN2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQP2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQR2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQT2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQV2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQX2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQZ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARB2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARD2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARF2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARH2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARJ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARL2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARQ2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ2" s="5" t="n"/>
+      <c r="ARR2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -17223,12 +17663,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APY3" s="5" t="inlineStr">
+      <c r="APY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARK3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARL3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARQ3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ3" s="5" t="n"/>
+      <c r="ARR3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -22811,12 +23471,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APY4" s="5" t="inlineStr">
+      <c r="APY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARL4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARQ4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ4" s="5" t="n"/>
+      <c r="ARR4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -28399,12 +29279,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APY5" s="5" t="inlineStr">
+      <c r="APY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQD5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQL5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQN5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQP5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQR5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQT5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQV5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQX5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQZ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARB5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARD5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARF5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARH5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARJ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARL5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARQ5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ5" s="5" t="n"/>
+      <c r="ARR5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -33987,12 +35087,232 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="APY6" s="5" t="inlineStr">
+      <c r="APY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="APZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQD6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQL6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQN6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQP6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQR6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQT6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQV6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQX6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQZ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARB6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARD6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARF6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARH6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARJ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARL6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARQ6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ6" s="5" t="n"/>
+      <c r="ARR6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -39575,12 +40895,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APY7" s="5" t="inlineStr">
+      <c r="APY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARL7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARQ7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ7" s="5" t="n"/>
+      <c r="ARR7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -45163,12 +46703,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APY8" s="5" t="inlineStr">
+      <c r="APY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQK8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQO8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQS8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQW8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AQZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARA8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARE8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARI8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARL8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARQ8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ8" s="5" t="n"/>
+      <c r="ARR8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -50751,12 +52511,232 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="APY9" s="5" t="inlineStr">
+      <c r="APY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="APZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AQZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARK9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARL9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARQ9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="APZ9" s="5" t="n"/>
+      <c r="ARR9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat(module_pour_excel, utils): modify apply_method_on_some_sheets to allow to choose some sheets. Write also a display function to see the completion of the run.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:ARR9"/>
+  <dimension ref="A1:ASD9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F4 E1"/>
@@ -6273,6 +6273,66 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="ARQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ART1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARU1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARV1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ARW1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ARX1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="ARY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="ARZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="ASA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="ASB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -12075,12 +12135,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ARQ2" s="5" t="inlineStr">
+      <c r="ARQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ART2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARU2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARV2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARX2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASC2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR2" s="5" t="n"/>
+      <c r="ASD2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -17883,12 +18003,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ARQ3" s="5" t="inlineStr">
+      <c r="ARQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ART3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARU3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARV3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARW3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARX3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASC3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR3" s="5" t="n"/>
+      <c r="ASD3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -23691,12 +23871,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ARQ4" s="5" t="inlineStr">
+      <c r="ARQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ART4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARU4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARV4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARX4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASC4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR4" s="5" t="n"/>
+      <c r="ASD4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -29499,12 +29739,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ARQ5" s="5" t="inlineStr">
+      <c r="ARQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ART5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARU5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARV5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARX5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASC5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR5" s="5" t="n"/>
+      <c r="ASD5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -35307,12 +35607,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="ARQ6" s="5" t="inlineStr">
+      <c r="ARQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ART6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARU6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARV6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARX6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASC6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR6" s="5" t="n"/>
+      <c r="ASD6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -41115,12 +41475,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ARQ7" s="5" t="inlineStr">
+      <c r="ARQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ART7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARU7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARV7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARX7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASC7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR7" s="5" t="n"/>
+      <c r="ASD7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -46923,12 +47343,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ARQ8" s="5" t="inlineStr">
+      <c r="ARQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ART8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARU8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARV8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ARX8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="ASB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASC8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR8" s="5" t="n"/>
+      <c r="ASD8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -52731,12 +53211,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="ARQ9" s="5" t="inlineStr">
+      <c r="ARQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ART9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARU9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARV9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARW9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARX9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ARZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="ASC9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="ARR9" s="5" t="n"/>
+      <c r="ASD9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
feat(xlspython): add a command keepcols (analogous to deletecols) but here we enter command we want to keep
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AXN9"/>
+  <dimension ref="A1:AXR9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -6926,6 +6926,26 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AXM1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AXN1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AXO1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AXP1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -13488,12 +13508,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXM2" s="5" t="inlineStr">
+      <c r="AXM2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXN2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXP2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXQ2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN2" s="5" t="n"/>
+      <c r="AXR2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -20056,12 +20096,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXM3" s="5" t="inlineStr">
+      <c r="AXM3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXN3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXO3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXP3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXQ3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN3" s="5" t="n"/>
+      <c r="AXR3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -26624,12 +26684,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXM4" s="5" t="inlineStr">
+      <c r="AXM4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXN4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXP4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXQ4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN4" s="5" t="n"/>
+      <c r="AXR4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -33192,12 +33272,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXM5" s="5" t="inlineStr">
+      <c r="AXM5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXN5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXP5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXQ5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN5" s="5" t="n"/>
+      <c r="AXR5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -39760,12 +39860,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXM6" s="5" t="inlineStr">
+      <c r="AXM6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXN6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXP6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXQ6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN6" s="5" t="n"/>
+      <c r="AXR6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -46328,12 +46448,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXM7" s="5" t="inlineStr">
+      <c r="AXM7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXN7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXP7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXQ7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN7" s="5" t="n"/>
+      <c r="AXR7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -52896,12 +53036,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXM8" s="5" t="inlineStr">
+      <c r="AXM8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXN8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXP8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXQ8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN8" s="5" t="n"/>
+      <c r="AXR8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -59464,12 +59624,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXM9" s="5" t="inlineStr">
+      <c r="AXM9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXN9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXO9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXP9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXQ9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXN9" s="5" t="n"/>
+      <c r="AXR9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
factor(architecture): modification of folders of the software
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AXR9"/>
+  <dimension ref="A1:AXV9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -6946,6 +6946,26 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AXQ1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AXR1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="AXS1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="AXT1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -13528,12 +13548,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXQ2" s="5" t="inlineStr">
+      <c r="AXQ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXR2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXT2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXU2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR2" s="5" t="n"/>
+      <c r="AXV2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -20116,12 +20156,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXQ3" s="5" t="inlineStr">
+      <c r="AXQ3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXR3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXS3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXT3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXU3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR3" s="5" t="n"/>
+      <c r="AXV3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -26704,12 +26764,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXQ4" s="5" t="inlineStr">
+      <c r="AXQ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXR4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXT4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXU4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR4" s="5" t="n"/>
+      <c r="AXV4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -33292,12 +33372,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXQ5" s="5" t="inlineStr">
+      <c r="AXQ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXR5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXT5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXU5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR5" s="5" t="n"/>
+      <c r="AXV5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -39880,12 +39980,32 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AXQ6" s="5" t="inlineStr">
+      <c r="AXQ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXR6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXT6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXU6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR6" s="5" t="n"/>
+      <c r="AXV6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -46468,12 +46588,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXQ7" s="5" t="inlineStr">
+      <c r="AXQ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXR7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXT7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXU7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR7" s="5" t="n"/>
+      <c r="AXV7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -53056,12 +53196,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXQ8" s="5" t="inlineStr">
+      <c r="AXQ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXR8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AXT8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXU8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR8" s="5" t="n"/>
+      <c r="AXV8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -59644,12 +59804,32 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AXQ9" s="5" t="inlineStr">
+      <c r="AXQ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXR9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXS9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXT9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AXU9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AXR9" s="5" t="n"/>
+      <c r="AXV9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>

<commit_message>
factor(all): apply single unique responsability principle to get smallest coherent classes
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_create_one_column.xlsx
+++ b/fichiers_xls/test_create_one_column.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AZZ9"/>
+  <dimension ref="A1:BAL9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -7246,6 +7246,66 @@
           <t>Dulcinée</t>
         </is>
       </c>
+      <c r="AZY1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="AZZ1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="BAA1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="BAB1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="BAC1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="BAD1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="BAE1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="BAF1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
+      <c r="BAG1" s="3" t="inlineStr">
+        <is>
+          <t>Alain</t>
+        </is>
+      </c>
+      <c r="BAH1" s="3" t="inlineStr">
+        <is>
+          <t>Henri</t>
+        </is>
+      </c>
+      <c r="BAI1" s="3" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="BAJ1" s="3" t="inlineStr">
+        <is>
+          <t>Dulcinée</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" s="4">
       <c r="A2" s="5" t="inlineStr">
@@ -7338,64 +7398,19 @@
           <t>X</t>
         </is>
       </c>
-      <c r="BI2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
       <c r="BJ2" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BK2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BL2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BM2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN2" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BO2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BP2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BQ2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR2" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BS2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BT2" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU2" s="3" t="inlineStr">
@@ -13918,12 +13933,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AZY2" s="5" t="inlineStr">
+      <c r="AZY2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AZZ2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAB2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAC2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAD2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAF2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAG2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAH2" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAJ2" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAK2" s="5" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ2" s="5" t="n"/>
+      <c r="BAL2" s="5" t="n"/>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -14088,62 +14163,32 @@
       </c>
       <c r="BI3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BJ3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BK3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BL3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BM3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BN3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BO3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BP3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BQ3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BR3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BS3" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BT3" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU3" s="3" t="inlineStr">
@@ -20666,12 +20711,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AZY3" s="5" t="inlineStr">
+      <c r="AZY3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AZZ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAA3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAB3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAC3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAD3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAE3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAF3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAG3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAH3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAI3" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAJ3" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAK3" s="5" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ3" s="5" t="n"/>
+      <c r="BAL3" s="5" t="n"/>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -20976,62 +21081,62 @@
       </c>
       <c r="BI4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BJ4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BK4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BL4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BM4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BO4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BP4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BQ4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BS4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BT4" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU4" s="3" t="inlineStr">
@@ -27554,12 +27659,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AZY4" s="5" t="inlineStr">
+      <c r="AZY4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AZZ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAB4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAC4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAD4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAF4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAG4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAH4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAJ4" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAK4" s="5" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ4" s="5" t="n"/>
+      <c r="BAL4" s="5" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -27652,64 +27817,19 @@
           <t>X</t>
         </is>
       </c>
-      <c r="BI5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
       <c r="BJ5" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BK5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BL5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BM5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN5" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BO5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BP5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BQ5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR5" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BS5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BT5" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU5" s="3" t="inlineStr">
@@ -34232,12 +34352,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AZY5" s="5" t="inlineStr">
+      <c r="AZY5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AZZ5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAB5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAC5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAD5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAF5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAG5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAH5" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAJ5" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAK5" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ5" s="5" t="n"/>
+      <c r="BAL5" s="5" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -34330,64 +34510,19 @@
           <t>X</t>
         </is>
       </c>
-      <c r="BI6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
       <c r="BJ6" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BK6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BL6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BM6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN6" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BO6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BP6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BQ6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR6" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BS6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
-        </is>
-      </c>
-      <c r="BT6" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU6" s="3" t="inlineStr">
@@ -40910,12 +41045,72 @@
           <t>NON</t>
         </is>
       </c>
-      <c r="AZY6" s="5" t="inlineStr">
+      <c r="AZY6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="AZZ6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAB6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAC6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAD6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAF6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAG6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAH6" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAJ6" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAK6" s="5" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ6" s="5" t="n"/>
+      <c r="BAL6" s="5" t="n"/>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -41220,62 +41415,62 @@
       </c>
       <c r="BI7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BJ7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BK7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BL7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BM7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BO7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BP7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BQ7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BS7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BT7" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU7" s="3" t="inlineStr">
@@ -47798,12 +47993,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AZY7" s="5" t="inlineStr">
+      <c r="AZY7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AZZ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAB7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAC7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAD7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAF7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAG7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAH7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAJ7" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAK7" s="5" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ7" s="5" t="n"/>
+      <c r="BAL7" s="5" t="n"/>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
@@ -48038,62 +48293,47 @@
       </c>
       <c r="BI8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BJ8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BK8" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BL8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BM8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BO8" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BP8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BQ8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
-        </is>
-      </c>
-      <c r="BS8" s="3" t="inlineStr">
-        <is>
-          <t>NON</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BT8" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU8" s="3" t="inlineStr">
@@ -54616,12 +54856,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AZY8" s="5" t="inlineStr">
+      <c r="AZY8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AZZ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAB8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAC8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAD8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAF8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAG8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAH8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI8" s="3" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="BAJ8" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAK8" s="5" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ8" s="5" t="n"/>
+      <c r="BAL8" s="5" t="n"/>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -54926,62 +55226,62 @@
       </c>
       <c r="BI9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BJ9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BK9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BL9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BM9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BN9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BO9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BP9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BQ9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BR9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BS9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BT9" s="3" t="inlineStr">
         <is>
-          <t>OUI</t>
+          <t>X</t>
         </is>
       </c>
       <c r="BU9" s="3" t="inlineStr">
@@ -61504,12 +61804,72 @@
           <t>OUI</t>
         </is>
       </c>
-      <c r="AZY9" s="5" t="inlineStr">
+      <c r="AZY9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="AZZ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAA9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAB9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAC9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAD9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAE9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAF9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAG9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAH9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAI9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAJ9" s="3" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="BAK9" s="5" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="AZZ9" s="5" t="n"/>
+      <c r="BAL9" s="5" t="n"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="4"/>
   </sheetData>

</xml_diff>